<commit_message>
Get Empty Holes After Removing Peg
</commit_message>
<xml_diff>
--- a/simulation.xlsx
+++ b/simulation.xlsx
@@ -45,7 +45,7 @@
     <t>G</t>
   </si>
   <si>
-    <t>F3,B3,D1,D5</t>
+    <t>F3,B3,D5,D1</t>
   </si>
 </sst>
 </file>
@@ -389,21 +389,24 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -415,9 +418,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -723,7 +723,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -782,7 +782,7 @@
       <c r="D3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="18" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="7" t="s">
@@ -824,7 +824,7 @@
       <c r="B5" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="18" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -836,7 +836,7 @@
       <c r="F5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="27" t="s">
+      <c r="G5" s="18" t="s">
         <v>0</v>
       </c>
       <c r="H5" s="10" t="s">
@@ -878,7 +878,7 @@
       <c r="D7" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="18" t="s">
         <v>0</v>
       </c>
       <c r="F7" s="7" t="s">
@@ -919,23 +919,23 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="22"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="23"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="24"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="24"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="26"/>
+      <c r="A11" s="25"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Most part of completed but duplicate case parent id should be fixed
</commit_message>
<xml_diff>
--- a/simulation.xlsx
+++ b/simulation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="15">
   <si>
     <t>x</t>
   </si>
@@ -60,14 +60,14 @@
     <t>F3,E3</t>
   </si>
   <si>
-    <t>F2,B2,D4</t>
+    <t>…</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,6 +109,14 @@
       <charset val="162"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -358,7 +366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -443,6 +451,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -745,10 +759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:Z16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -757,9 +771,11 @@
     <col min="2" max="8" width="1.90625" customWidth="1"/>
     <col min="10" max="10" width="2.26953125" customWidth="1"/>
     <col min="11" max="17" width="1.90625" customWidth="1"/>
+    <col min="19" max="19" width="2.26953125" customWidth="1"/>
+    <col min="20" max="26" width="1.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" s="12" t="s">
         <v>2</v>
       </c>
@@ -802,8 +818,29 @@
       <c r="Q1" s="12" t="s">
         <v>8</v>
       </c>
+      <c r="T1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="U1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="V1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="W1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="X1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z1" s="12" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="11">
         <v>0</v>
       </c>
@@ -836,8 +873,24 @@
       </c>
       <c r="P2" s="2"/>
       <c r="Q2" s="4"/>
+      <c r="S2" s="11">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="4"/>
     </row>
-    <row r="3" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="11">
         <v>1</v>
       </c>
@@ -863,15 +916,31 @@
         <v>0</v>
       </c>
       <c r="N3" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="O3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="O3" s="18" t="s">
         <v>0</v>
       </c>
       <c r="P3" s="6"/>
       <c r="Q3" s="8"/>
+      <c r="S3" s="11">
+        <v>1</v>
+      </c>
+      <c r="T3" s="5"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="W3" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="X3" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="8"/>
     </row>
-    <row r="4" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="11">
         <v>2</v>
       </c>
@@ -902,26 +971,50 @@
       <c r="K4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="L4" s="18" t="s">
+      <c r="L4" s="7" t="s">
         <v>0</v>
       </c>
       <c r="M4" s="7" t="s">
         <v>0</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="P4" s="18" t="s">
+      <c r="P4" s="7" t="s">
         <v>0</v>
       </c>
       <c r="Q4" s="10" t="s">
         <v>0</v>
       </c>
+      <c r="S4" s="11">
+        <v>2</v>
+      </c>
+      <c r="T4" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="U4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="V4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="W4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="X4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="10" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="11">
         <v>3</v>
       </c>
@@ -955,23 +1048,50 @@
       <c r="L5" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="M5" s="18" t="s">
         <v>0</v>
       </c>
       <c r="N5" s="7" t="s">
         <v>0</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P5" s="19" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q5" s="10" t="s">
         <v>0</v>
       </c>
+      <c r="R5" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="S5" s="11">
+        <v>3</v>
+      </c>
+      <c r="T5" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="U5" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="V5" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="W5" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="X5" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="10" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="11">
         <v>4</v>
       </c>
@@ -1008,7 +1128,7 @@
       <c r="M6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="N6" s="18" t="s">
+      <c r="N6" s="7" t="s">
         <v>0</v>
       </c>
       <c r="O6" s="7" t="s">
@@ -1020,8 +1140,32 @@
       <c r="Q6" s="10" t="s">
         <v>0</v>
       </c>
+      <c r="S6" s="11">
+        <v>4</v>
+      </c>
+      <c r="T6" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="U6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="V6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="W6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="X6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="10" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="11">
         <v>5</v>
       </c>
@@ -1049,13 +1193,29 @@
       <c r="N7" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="O7" s="7" t="s">
+      <c r="O7" s="18" t="s">
         <v>0</v>
       </c>
       <c r="P7" s="6"/>
       <c r="Q7" s="8"/>
+      <c r="S7" s="11">
+        <v>5</v>
+      </c>
+      <c r="T7" s="5"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="W7" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="X7" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="8"/>
     </row>
-    <row r="8" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="13">
         <v>6</v>
       </c>
@@ -1088,8 +1248,24 @@
       </c>
       <c r="P8" s="15"/>
       <c r="Q8" s="17"/>
+      <c r="S8" s="13">
+        <v>6</v>
+      </c>
+      <c r="T8" s="14"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="W8" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="X8" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="15"/>
+      <c r="Z8" s="17"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
         <v>9</v>
       </c>
@@ -1101,7 +1277,7 @@
       <c r="G9" s="21"/>
       <c r="H9" s="22"/>
       <c r="J9" s="20" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="K9" s="21"/>
       <c r="L9" s="21"/>
@@ -1110,8 +1286,18 @@
       <c r="O9" s="21"/>
       <c r="P9" s="21"/>
       <c r="Q9" s="22"/>
+      <c r="S9" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="T9" s="21"/>
+      <c r="U9" s="21"/>
+      <c r="V9" s="21"/>
+      <c r="W9" s="21"/>
+      <c r="X9" s="21"/>
+      <c r="Y9" s="21"/>
+      <c r="Z9" s="22"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" s="23"/>
       <c r="B10" s="24"/>
       <c r="C10" s="24"/>
@@ -1128,8 +1314,16 @@
       <c r="O10" s="24"/>
       <c r="P10" s="24"/>
       <c r="Q10" s="25"/>
+      <c r="S10" s="23"/>
+      <c r="T10" s="24"/>
+      <c r="U10" s="24"/>
+      <c r="V10" s="24"/>
+      <c r="W10" s="24"/>
+      <c r="X10" s="24"/>
+      <c r="Y10" s="24"/>
+      <c r="Z10" s="25"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11" s="26"/>
       <c r="B11" s="27"/>
       <c r="C11" s="27"/>
@@ -1146,31 +1340,64 @@
       <c r="O11" s="27"/>
       <c r="P11" s="27"/>
       <c r="Q11" s="28"/>
+      <c r="S11" s="26"/>
+      <c r="T11" s="27"/>
+      <c r="U11" s="27"/>
+      <c r="V11" s="27"/>
+      <c r="W11" s="27"/>
+      <c r="X11" s="27"/>
+      <c r="Y11" s="27"/>
+      <c r="Z11" s="28"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
+      <c r="J13" t="s">
+        <v>10</v>
+      </c>
+      <c r="S13" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>11</v>
       </c>
+      <c r="J14" t="s">
+        <v>11</v>
+      </c>
+      <c r="S14" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>12</v>
       </c>
+      <c r="J15" t="s">
+        <v>12</v>
+      </c>
+      <c r="S15" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>13</v>
       </c>
+      <c r="J16" t="s">
+        <v>13</v>
+      </c>
+      <c r="S16" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A9:H11"/>
     <mergeCell ref="J9:Q11"/>
+    <mergeCell ref="S9:Z11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Migrate to Artificial Intelligence Modern Approach(aima) solution
</commit_message>
<xml_diff>
--- a/simulation.xlsx
+++ b/simulation.xlsx
@@ -422,6 +422,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -448,12 +454,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1104,7 +1104,7 @@
       <c r="D5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="21" t="s">
         <v>1</v>
       </c>
       <c r="F5" s="7" t="s">
@@ -1140,7 +1140,7 @@
       <c r="Q5" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="R5" s="29"/>
+      <c r="R5" s="20"/>
       <c r="S5" s="11">
         <v>3</v>
       </c>
@@ -1150,16 +1150,16 @@
       <c r="U5" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="V5" s="30" t="s">
+      <c r="V5" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="W5" s="30" t="s">
+      <c r="W5" s="21" t="s">
         <v>1</v>
       </c>
       <c r="X5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="Y5" s="30" t="s">
+      <c r="Y5" s="21" t="s">
         <v>1</v>
       </c>
       <c r="Z5" s="10" t="s">
@@ -1174,16 +1174,16 @@
       <c r="AD5" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="AE5" s="30" t="s">
+      <c r="AE5" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="AF5" s="30" t="s">
+      <c r="AF5" s="21" t="s">
         <v>1</v>
       </c>
       <c r="AG5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="AH5" s="30" t="s">
+      <c r="AH5" s="21" t="s">
         <v>1</v>
       </c>
       <c r="AI5" s="10" t="s">
@@ -1421,114 +1421,114 @@
       <c r="AI8" s="17"/>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="22"/>
-      <c r="J9" s="20" t="s">
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="24"/>
+      <c r="J9" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="22"/>
-      <c r="S9" s="20" t="s">
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="24"/>
+      <c r="S9" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="T9" s="21"/>
-      <c r="U9" s="21"/>
-      <c r="V9" s="21"/>
-      <c r="W9" s="21"/>
-      <c r="X9" s="21"/>
-      <c r="Y9" s="21"/>
-      <c r="Z9" s="22"/>
-      <c r="AB9" s="20" t="s">
+      <c r="T9" s="23"/>
+      <c r="U9" s="23"/>
+      <c r="V9" s="23"/>
+      <c r="W9" s="23"/>
+      <c r="X9" s="23"/>
+      <c r="Y9" s="23"/>
+      <c r="Z9" s="24"/>
+      <c r="AB9" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="AC9" s="21"/>
-      <c r="AD9" s="21"/>
-      <c r="AE9" s="21"/>
-      <c r="AF9" s="21"/>
-      <c r="AG9" s="21"/>
-      <c r="AH9" s="21"/>
-      <c r="AI9" s="22"/>
+      <c r="AC9" s="23"/>
+      <c r="AD9" s="23"/>
+      <c r="AE9" s="23"/>
+      <c r="AF9" s="23"/>
+      <c r="AG9" s="23"/>
+      <c r="AH9" s="23"/>
+      <c r="AI9" s="24"/>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A10" s="23"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="25"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="24"/>
-      <c r="O10" s="24"/>
-      <c r="P10" s="24"/>
-      <c r="Q10" s="25"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="24"/>
-      <c r="U10" s="24"/>
-      <c r="V10" s="24"/>
-      <c r="W10" s="24"/>
-      <c r="X10" s="24"/>
-      <c r="Y10" s="24"/>
-      <c r="Z10" s="25"/>
-      <c r="AB10" s="23"/>
-      <c r="AC10" s="24"/>
-      <c r="AD10" s="24"/>
-      <c r="AE10" s="24"/>
-      <c r="AF10" s="24"/>
-      <c r="AG10" s="24"/>
-      <c r="AH10" s="24"/>
-      <c r="AI10" s="25"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="27"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="26"/>
+      <c r="O10" s="26"/>
+      <c r="P10" s="26"/>
+      <c r="Q10" s="27"/>
+      <c r="S10" s="25"/>
+      <c r="T10" s="26"/>
+      <c r="U10" s="26"/>
+      <c r="V10" s="26"/>
+      <c r="W10" s="26"/>
+      <c r="X10" s="26"/>
+      <c r="Y10" s="26"/>
+      <c r="Z10" s="27"/>
+      <c r="AB10" s="25"/>
+      <c r="AC10" s="26"/>
+      <c r="AD10" s="26"/>
+      <c r="AE10" s="26"/>
+      <c r="AF10" s="26"/>
+      <c r="AG10" s="26"/>
+      <c r="AH10" s="26"/>
+      <c r="AI10" s="27"/>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A11" s="26"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="28"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="27"/>
-      <c r="N11" s="27"/>
-      <c r="O11" s="27"/>
-      <c r="P11" s="27"/>
-      <c r="Q11" s="28"/>
-      <c r="S11" s="26"/>
-      <c r="T11" s="27"/>
-      <c r="U11" s="27"/>
-      <c r="V11" s="27"/>
-      <c r="W11" s="27"/>
-      <c r="X11" s="27"/>
-      <c r="Y11" s="27"/>
-      <c r="Z11" s="28"/>
-      <c r="AB11" s="26"/>
-      <c r="AC11" s="27"/>
-      <c r="AD11" s="27"/>
-      <c r="AE11" s="27"/>
-      <c r="AF11" s="27"/>
-      <c r="AG11" s="27"/>
-      <c r="AH11" s="27"/>
-      <c r="AI11" s="28"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="30"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="29"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="29"/>
+      <c r="Q11" s="30"/>
+      <c r="S11" s="28"/>
+      <c r="T11" s="29"/>
+      <c r="U11" s="29"/>
+      <c r="V11" s="29"/>
+      <c r="W11" s="29"/>
+      <c r="X11" s="29"/>
+      <c r="Y11" s="29"/>
+      <c r="Z11" s="30"/>
+      <c r="AB11" s="28"/>
+      <c r="AC11" s="29"/>
+      <c r="AD11" s="29"/>
+      <c r="AE11" s="29"/>
+      <c r="AF11" s="29"/>
+      <c r="AG11" s="29"/>
+      <c r="AH11" s="29"/>
+      <c r="AI11" s="30"/>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A13" t="s">

</xml_diff>